<commit_message>
Fix rp weights for Markov truth case (and other cases)
</commit_message>
<xml_diff>
--- a/data/markov/Power_Demand.xlsx
+++ b/data/markov/Power_Demand.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\markov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7098EFB4-8B8D-4D2E-9699-AD781647DC35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80144F91-C16D-4BE7-B064-AE3F5C081DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="461" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="461" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Demand" sheetId="4" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>rp01</t>
   </si>
@@ -251,6 +251,12 @@
   </si>
   <si>
     <t>[MWh]</t>
+  </si>
+  <si>
+    <t>rp05</t>
+  </si>
+  <si>
+    <t>rp06</t>
   </si>
 </sst>
 </file>
@@ -790,7 +796,7 @@
   <dimension ref="B1:AB17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,59 +1264,193 @@
       <c r="R10" s="12">
         <v>1434.8910999999998</v>
       </c>
-      <c r="S10" s="12">
-        <v>1434.8910999999998</v>
-      </c>
-      <c r="T10" s="12">
-        <v>1434.8910999999998</v>
-      </c>
-      <c r="U10" s="12">
-        <v>1434.8910999999998</v>
-      </c>
-      <c r="V10" s="12">
-        <v>1434.8910999999998</v>
-      </c>
-      <c r="W10" s="12">
-        <v>1434.8910999999998</v>
-      </c>
-      <c r="X10" s="12">
-        <v>1434.8910999999998</v>
-      </c>
-      <c r="Y10" s="12">
-        <v>1434.8910999999998</v>
-      </c>
-      <c r="Z10" s="12">
-        <v>1434.8910999999998</v>
-      </c>
-      <c r="AA10" s="12">
-        <v>1434.8910999999998</v>
+      <c r="S10" s="9">
+        <v>1400</v>
+      </c>
+      <c r="T10" s="9">
+        <v>1350</v>
+      </c>
+      <c r="U10" s="9">
+        <v>1300</v>
+      </c>
+      <c r="V10" s="9">
+        <v>1250</v>
+      </c>
+      <c r="W10" s="9">
+        <v>1200</v>
+      </c>
+      <c r="X10" s="9">
+        <v>1150</v>
+      </c>
+      <c r="Y10" s="9">
+        <v>1100</v>
+      </c>
+      <c r="Z10" s="9">
+        <v>1050</v>
+      </c>
+      <c r="AA10" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="9">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="E11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="F11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="G11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="H11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="I11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="J11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="K11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="L11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="M11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="N11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="O11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="P11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="Q11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="R11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="S11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="T11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="U11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="V11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="W11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="X11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="Y11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="Z11" s="12">
+        <v>890.38409999999999</v>
+      </c>
+      <c r="AA11" s="12">
+        <v>890.38409999999999</v>
       </c>
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="11"/>
-      <c r="W12" s="11"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="11"/>
-      <c r="Z12" s="11"/>
-      <c r="AA12" s="11"/>
+      <c r="B12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="9">
+        <v>1000</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1050</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1100</v>
+      </c>
+      <c r="G12" s="9">
+        <v>1150</v>
+      </c>
+      <c r="H12" s="9">
+        <v>1200</v>
+      </c>
+      <c r="I12" s="9">
+        <v>1250</v>
+      </c>
+      <c r="J12" s="9">
+        <v>1300</v>
+      </c>
+      <c r="K12" s="9">
+        <v>1350</v>
+      </c>
+      <c r="L12" s="9">
+        <v>1400</v>
+      </c>
+      <c r="M12" s="12">
+        <v>1434.8910999999998</v>
+      </c>
+      <c r="N12" s="12">
+        <v>1434.8910999999998</v>
+      </c>
+      <c r="O12" s="12">
+        <v>1434.8910999999998</v>
+      </c>
+      <c r="P12" s="12">
+        <v>1434.8910999999998</v>
+      </c>
+      <c r="Q12" s="12">
+        <v>1434.8910999999998</v>
+      </c>
+      <c r="R12" s="12">
+        <v>1434.8910999999998</v>
+      </c>
+      <c r="S12" s="12">
+        <v>1434.8910999999998</v>
+      </c>
+      <c r="T12" s="12">
+        <v>1434.8910999999998</v>
+      </c>
+      <c r="U12" s="12">
+        <v>1434.8910999999998</v>
+      </c>
+      <c r="V12" s="12">
+        <v>1434.8910999999998</v>
+      </c>
+      <c r="W12" s="12">
+        <v>1434.8910999999998</v>
+      </c>
+      <c r="X12" s="12">
+        <v>1434.8910999999998</v>
+      </c>
+      <c r="Y12" s="12">
+        <v>1434.8910999999998</v>
+      </c>
+      <c r="Z12" s="12">
+        <v>1434.8910999999998</v>
+      </c>
+      <c r="AA12" s="12">
+        <v>1434.8910999999998</v>
+      </c>
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.25">
       <c r="D16" s="11"/>
@@ -1821,39 +1961,39 @@
       </c>
       <c r="U19" s="11">
         <f>SUM('Power Demand'!S10:S10)</f>
-        <v>1434.8910999999998</v>
+        <v>1400</v>
       </c>
       <c r="V19" s="11">
         <f>SUM('Power Demand'!T10:T10)</f>
-        <v>1434.8910999999998</v>
+        <v>1350</v>
       </c>
       <c r="W19" s="11">
         <f>SUM('Power Demand'!U10:U10)</f>
-        <v>1434.8910999999998</v>
+        <v>1300</v>
       </c>
       <c r="X19" s="11">
         <f>SUM('Power Demand'!V10:V10)</f>
-        <v>1434.8910999999998</v>
+        <v>1250</v>
       </c>
       <c r="Y19" s="11">
         <f>SUM('Power Demand'!W10:W10)</f>
-        <v>1434.8910999999998</v>
+        <v>1200</v>
       </c>
       <c r="Z19" s="11">
         <f>SUM('Power Demand'!X10:X10)</f>
-        <v>1434.8910999999998</v>
+        <v>1150</v>
       </c>
       <c r="AA19" s="11">
         <f>SUM('Power Demand'!Y10:Y10)</f>
-        <v>1434.8910999999998</v>
+        <v>1100</v>
       </c>
       <c r="AB19" s="11">
         <f>SUM('Power Demand'!Z10:Z10)</f>
-        <v>1434.8910999999998</v>
+        <v>1050</v>
       </c>
       <c r="AC19" s="11">
         <f>SUM('Power Demand'!AA10:AA10)</f>
-        <v>1434.8910999999998</v>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -1862,9 +2002,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2014,26 +2157,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2057,9 +2189,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adjust markov case study to avoid PNS
Reduce Demand by 1%
Deactivate 2nd Reserve, increase PENS cost
Move production capability from OCGT to CCGT
</commit_message>
<xml_diff>
--- a/data/markov/Power_Demand.xlsx
+++ b/data/markov/Power_Demand.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\markov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE50266-265D-440E-9936-600CDDAAE6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF83D01F-54D3-4569-9E9D-BCB42695FC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" tabRatio="461" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="461" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioA" sheetId="4" r:id="rId1"/>
@@ -899,10 +899,10 @@
   <dimension ref="B1:AD14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="7" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15:AD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,76 +1347,76 @@
         <v>56</v>
       </c>
       <c r="G8" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="H8" s="11">
-        <v>1411.2168826086956</v>
+        <v>1397.1047137826088</v>
       </c>
       <c r="I8" s="11">
-        <v>1387.5426652173912</v>
+        <v>1373.6672385652173</v>
       </c>
       <c r="J8" s="11">
-        <v>1363.868447826087</v>
+        <v>1350.2297633478261</v>
       </c>
       <c r="K8" s="11">
-        <v>1340.1942304347826</v>
+        <v>1326.7922881304348</v>
       </c>
       <c r="L8" s="11">
-        <v>1316.5200130434782</v>
+        <v>1303.3548129130434</v>
       </c>
       <c r="M8" s="11">
-        <v>1292.8457956521738</v>
+        <v>1279.9173376956521</v>
       </c>
       <c r="N8" s="11">
-        <v>1269.1715782608696</v>
+        <v>1256.4798624782609</v>
       </c>
       <c r="O8" s="11">
-        <v>1245.497360869565</v>
+        <v>1233.0423872608694</v>
       </c>
       <c r="P8" s="11">
-        <v>1221.8231434782608</v>
+        <v>1209.6049120434782</v>
       </c>
       <c r="Q8" s="11">
-        <v>1198.1489260869564</v>
+        <v>1186.1674368260869</v>
       </c>
       <c r="R8" s="11">
-        <v>1174.4747086956522</v>
+        <v>1162.7299616086957</v>
       </c>
       <c r="S8" s="11">
-        <v>1150.8004913043478</v>
+        <v>1139.2924863913042</v>
       </c>
       <c r="T8" s="11">
-        <v>1127.1262739130434</v>
+        <v>1115.855011173913</v>
       </c>
       <c r="U8" s="11">
-        <v>1103.452056521739</v>
+        <v>1092.4175359565215</v>
       </c>
       <c r="V8" s="11">
-        <v>1079.7778391304346</v>
+        <v>1068.9800607391303</v>
       </c>
       <c r="W8" s="11">
-        <v>1056.1036217391302</v>
+        <v>1045.5425855217388</v>
       </c>
       <c r="X8" s="11">
-        <v>1032.429404347826</v>
+        <v>1022.1051103043477</v>
       </c>
       <c r="Y8" s="11">
-        <v>1008.7551869565217</v>
+        <v>998.66763508695647</v>
       </c>
       <c r="Z8" s="11">
-        <v>985.0809695652174</v>
+        <v>975.23015986956523</v>
       </c>
       <c r="AA8" s="11">
-        <v>961.40675217391299</v>
+        <v>951.79268465217388</v>
       </c>
       <c r="AB8" s="11">
-        <v>937.73253478260858</v>
+        <v>928.35520943478252</v>
       </c>
       <c r="AC8" s="11">
-        <v>914.0583173913044</v>
+        <v>904.9177342173914</v>
       </c>
       <c r="AD8" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.25">
@@ -1434,76 +1434,76 @@
         <v>56</v>
       </c>
       <c r="G9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="H9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="I9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="J9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="K9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="L9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="M9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="N9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="O9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="P9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="Q9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="R9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="S9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="T9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="U9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="V9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="W9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="X9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="Y9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="Z9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="AA9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="AB9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="AC9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="AD9" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.25">
@@ -1521,76 +1521,76 @@
         <v>56</v>
       </c>
       <c r="G10" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="H10" s="11">
-        <v>914.0583173913044</v>
+        <v>904.9177342173914</v>
       </c>
       <c r="I10" s="11">
-        <v>937.73253478260858</v>
+        <v>928.35520943478252</v>
       </c>
       <c r="J10" s="11">
-        <v>961.40675217391299</v>
+        <v>951.79268465217388</v>
       </c>
       <c r="K10" s="11">
-        <v>985.08096956521729</v>
+        <v>975.23015986956511</v>
       </c>
       <c r="L10" s="11">
-        <v>1008.7551869565216</v>
+        <v>998.66763508695635</v>
       </c>
       <c r="M10" s="11">
-        <v>1032.429404347826</v>
+        <v>1022.1051103043477</v>
       </c>
       <c r="N10" s="11">
-        <v>1056.1036217391302</v>
+        <v>1045.5425855217388</v>
       </c>
       <c r="O10" s="11">
-        <v>1079.7778391304346</v>
+        <v>1068.9800607391303</v>
       </c>
       <c r="P10" s="11">
-        <v>1103.452056521739</v>
+        <v>1092.4175359565215</v>
       </c>
       <c r="Q10" s="11">
-        <v>1127.1262739130434</v>
+        <v>1115.855011173913</v>
       </c>
       <c r="R10" s="11">
-        <v>1150.8004913043476</v>
+        <v>1139.292486391304</v>
       </c>
       <c r="S10" s="11">
-        <v>1174.4747086956522</v>
+        <v>1162.7299616086957</v>
       </c>
       <c r="T10" s="11">
-        <v>1198.1489260869564</v>
+        <v>1186.1674368260869</v>
       </c>
       <c r="U10" s="11">
-        <v>1221.8231434782608</v>
+        <v>1209.6049120434782</v>
       </c>
       <c r="V10" s="11">
-        <v>1245.497360869565</v>
+        <v>1233.0423872608694</v>
       </c>
       <c r="W10" s="11">
-        <v>1269.1715782608694</v>
+        <v>1256.4798624782607</v>
       </c>
       <c r="X10" s="11">
-        <v>1292.8457956521738</v>
+        <v>1279.9173376956521</v>
       </c>
       <c r="Y10" s="11">
-        <v>1316.5200130434782</v>
+        <v>1303.3548129130434</v>
       </c>
       <c r="Z10" s="11">
-        <v>1340.1942304347824</v>
+        <v>1326.7922881304346</v>
       </c>
       <c r="AA10" s="11">
-        <v>1363.868447826087</v>
+        <v>1350.2297633478261</v>
       </c>
       <c r="AB10" s="11">
-        <v>1387.5426652173912</v>
+        <v>1373.6672385652173</v>
       </c>
       <c r="AC10" s="11">
-        <v>1411.2168826086956</v>
+        <v>1397.1047137826088</v>
       </c>
       <c r="AD10" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
     </row>
     <row r="11" spans="2:30" x14ac:dyDescent="0.25">
@@ -1608,76 +1608,76 @@
         <v>56</v>
       </c>
       <c r="G11" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="H11" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="I11" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="J11" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="K11" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="L11" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="M11" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="N11" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="O11" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="P11" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="Q11" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="R11" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="S11" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="T11" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="U11" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="V11" s="11">
-        <v>1400</v>
+        <v>1386</v>
       </c>
       <c r="W11" s="11">
-        <v>1350</v>
+        <v>1336.5</v>
       </c>
       <c r="X11" s="11">
-        <v>1300</v>
+        <v>1287</v>
       </c>
       <c r="Y11" s="11">
-        <v>1250</v>
+        <v>1237.5</v>
       </c>
       <c r="Z11" s="11">
-        <v>1200</v>
+        <v>1188</v>
       </c>
       <c r="AA11" s="11">
-        <v>1150</v>
+        <v>1138.5</v>
       </c>
       <c r="AB11" s="11">
-        <v>1100</v>
+        <v>1089</v>
       </c>
       <c r="AC11" s="11">
-        <v>1050</v>
+        <v>1039.5</v>
       </c>
       <c r="AD11" s="11">
-        <v>1000</v>
+        <v>990</v>
       </c>
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.25">
@@ -1695,76 +1695,76 @@
         <v>56</v>
       </c>
       <c r="G12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="H12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="I12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="J12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="K12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="L12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="M12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="N12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="O12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="P12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="Q12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="R12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="S12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="T12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="U12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="V12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="W12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="X12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="Y12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="Z12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="AA12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="AB12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="AC12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
       <c r="AD12" s="11">
-        <v>890.38409999999999</v>
+        <v>881.48025899999993</v>
       </c>
     </row>
     <row r="13" spans="2:30" x14ac:dyDescent="0.25">
@@ -1782,76 +1782,76 @@
         <v>56</v>
       </c>
       <c r="G13" s="11">
-        <v>1000</v>
+        <v>990</v>
       </c>
       <c r="H13" s="11">
-        <v>1050</v>
+        <v>1039.5</v>
       </c>
       <c r="I13" s="11">
-        <v>1100</v>
+        <v>1089</v>
       </c>
       <c r="J13" s="11">
-        <v>1150</v>
+        <v>1138.5</v>
       </c>
       <c r="K13" s="11">
-        <v>1200</v>
+        <v>1188</v>
       </c>
       <c r="L13" s="11">
-        <v>1250</v>
+        <v>1237.5</v>
       </c>
       <c r="M13" s="11">
-        <v>1300</v>
+        <v>1287</v>
       </c>
       <c r="N13" s="11">
-        <v>1350</v>
+        <v>1336.5</v>
       </c>
       <c r="O13" s="11">
-        <v>1400</v>
+        <v>1386</v>
       </c>
       <c r="P13" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="Q13" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="R13" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="S13" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="T13" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="U13" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="V13" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="W13" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="X13" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="Y13" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="Z13" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="AA13" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="AB13" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="AC13" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
       <c r="AD13" s="11">
-        <v>1434.8910999999998</v>
+        <v>1420.5421889999998</v>
       </c>
     </row>
     <row r="14" spans="2:30" x14ac:dyDescent="0.25">
@@ -1875,6 +1875,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2020,12 +2026,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2036,6 +2036,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2053,22 +2069,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Adapt illustrative case to reduce min up-/down-time
</commit_message>
<xml_diff>
--- a/data/markov/Power_Demand.xlsx
+++ b/data/markov/Power_Demand.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\markov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339749D1-73BD-4C21-9FFC-659294B5C72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE1EBAD-D1CB-4339-9985-494CAD1BF598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11790" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50205" yWindow="-21690" windowWidth="19410" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioA" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -329,7 +329,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.00000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -456,7 +456,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2298,11 +2298,11 @@
   </sheetPr>
   <dimension ref="A1:AD18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="7" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3135,7 +3135,7 @@
         <v>1000</v>
       </c>
       <c r="I11" s="14">
-        <f t="shared" ref="I11:AD12" si="3">IF(I2="x",H11-($G$1-$I$1)/COUNTIF($G$2:$AD$2,"x"),H11)</f>
+        <f t="shared" ref="I11:AD11" si="3">IF(I2="x",H11-($G$1-$I$1)/COUNTIF($G$2:$AD$2,"x"),H11)</f>
         <v>1000</v>
       </c>
       <c r="J11" s="14">
@@ -3290,7 +3290,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="14">
-        <f t="shared" ref="T12:AB12" si="5">IF(T2="x",U12-($I$1-$H$1)/COUNTIF($G$2:$AD$2,"x"),U12)</f>
+        <f t="shared" ref="T12:Y12" si="5">IF(T2="x",U12-($I$1-$H$1)/COUNTIF($G$2:$AD$2,"x"),U12)</f>
         <v>0</v>
       </c>
       <c r="U12" s="14">

</xml_diff>

<commit_message>
Increase min up-/down-time to also show non-binarities
</commit_message>
<xml_diff>
--- a/data/markov/Power_Demand.xlsx
+++ b/data/markov/Power_Demand.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\markov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE1EBAD-D1CB-4339-9985-494CAD1BF598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2221A390-4F10-43C5-88C7-C25949C06680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50205" yWindow="-21690" windowWidth="19410" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -825,16 +825,16 @@
                   <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>766.66666666666663</c:v>
+                  <c:v>733.33333333333326</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>533.33333333333326</c:v>
+                  <c:v>466.66666666666657</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>299.99999999999989</c:v>
+                  <c:v>199.99999999999989</c:v>
                 </c:pt>
                 <c:pt idx="96" formatCode="0">
-                  <c:v>66.666666666666544</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="97">
                   <c:v>0</c:v>
@@ -903,16 +903,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>66.666666666666544</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="120" formatCode="0">
-                  <c:v>299.99999999999989</c:v>
+                  <c:v>199.99999999999989</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>533.33333333333326</c:v>
+                  <c:v>466.66666666666657</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>766.66666666666663</c:v>
+                  <c:v>733.33333333333326</c:v>
                 </c:pt>
                 <c:pt idx="123">
                   <c:v>1000</c:v>
@@ -2302,7 +2302,7 @@
       <pane xSplit="2" ySplit="7" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2330,7 +2330,7 @@
         <v>0</v>
       </c>
       <c r="I1" s="1">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -3212,15 +3212,15 @@
       </c>
       <c r="AB11" s="14">
         <f t="shared" si="3"/>
-        <v>766.66666666666663</v>
+        <v>733.33333333333326</v>
       </c>
       <c r="AC11" s="14">
         <f t="shared" si="3"/>
-        <v>533.33333333333326</v>
+        <v>466.66666666666657</v>
       </c>
       <c r="AD11" s="14">
         <f t="shared" si="3"/>
-        <v>299.99999999999989</v>
+        <v>199.99999999999989</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.4">
@@ -3239,7 +3239,7 @@
       </c>
       <c r="G12" s="14">
         <f>MAX(AD11-($G$1-$I$1)/COUNTIF($G$2:$AD$2,"x"),0)</f>
-        <v>66.666666666666544</v>
+        <v>0</v>
       </c>
       <c r="H12" s="14">
         <f>MAX(G12-($G$1-$I$1)/COUNTIF($G$2:$AD$2,"x"),0)</f>
@@ -3331,7 +3331,7 @@
       </c>
       <c r="AD12" s="14">
         <f>G12</f>
-        <v>66.666666666666544</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.4">
@@ -3350,15 +3350,15 @@
       </c>
       <c r="G13" s="14">
         <f t="shared" ref="G13:AB13" si="6">IF(G2="a",H13-($G$1-$I$1)/COUNTIF($G$2:$AD$2,"a"),H13)</f>
-        <v>299.99999999999989</v>
+        <v>199.99999999999989</v>
       </c>
       <c r="H13" s="14">
         <f t="shared" si="6"/>
-        <v>533.33333333333326</v>
+        <v>466.66666666666657</v>
       </c>
       <c r="I13" s="14">
         <f t="shared" si="6"/>
-        <v>766.66666666666663</v>
+        <v>733.33333333333326</v>
       </c>
       <c r="J13" s="14">
         <f t="shared" si="6"/>
@@ -3942,23 +3942,23 @@
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B95">
-        <v>766.66666666666663</v>
+        <v>733.33333333333326</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B96">
-        <v>533.33333333333326</v>
+        <v>466.66666666666657</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B97">
-        <v>299.99999999999989</v>
+        <v>199.99999999999989</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B98" s="15" cm="1">
         <f t="array" ref="B98:B121">TRANSPOSE(ScenarioA!G12:AD12)</f>
-        <v>66.666666666666544</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.4">
@@ -4073,23 +4073,23 @@
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B121">
-        <v>66.666666666666544</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B122" s="15" cm="1">
         <f t="array" ref="B122:B145">TRANSPOSE(ScenarioA!G13:AD13)</f>
-        <v>299.99999999999989</v>
+        <v>199.99999999999989</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B123">
-        <v>533.33333333333326</v>
+        <v>466.66666666666657</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B124">
-        <v>766.66666666666663</v>
+        <v>733.33333333333326</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.4">

</xml_diff>